<commit_message>
Update Documentation : SVT OS Tick (Pictures) and Traceability Matrix Update
</commit_message>
<xml_diff>
--- a/documentation/1.0 Requirements/Traceability Matrix 0.0 OS Tick.xlsx
+++ b/documentation/1.0 Requirements/Traceability Matrix 0.0 OS Tick.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>Program</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Sergio,Esteban,Miguel</t>
+  </si>
+  <si>
+    <t>DSD 0.0 OS Tick.docx</t>
   </si>
 </sst>
 </file>
@@ -525,6 +528,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,9 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1433,9 +1436,9 @@
   </sheetPr>
   <dimension ref="A1:IF65363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" outlineLevelCol="1"/>
@@ -1468,9 +1471,9 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="21.6" customHeight="1" thickTop="1">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1485,9 +1488,9 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="18" t="s">
         <v>8</v>
       </c>
@@ -1502,9 +1505,9 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="18" t="s">
         <v>20</v>
       </c>
@@ -1517,9 +1520,9 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="45">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
@@ -1534,9 +1537,9 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="18" t="s">
         <v>5</v>
       </c>
@@ -1546,18 +1549,18 @@
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41" t="s">
+      <c r="H6" s="41"/>
+      <c r="I6" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="38" t="s">
+      <c r="J6" s="43"/>
+      <c r="K6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="39"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="1:12" s="6" customFormat="1" ht="16.5" thickTop="1">
       <c r="A7" s="16" t="s">
@@ -1640,12 +1643,14 @@
       <c r="F9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="32" t="s">
         <v>49</v>
       </c>
       <c r="K9" s="14" t="s">
@@ -1670,9 +1675,11 @@
         <v>51</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="32" t="s">
         <v>47</v>
       </c>
       <c r="J10" s="15"/>
@@ -1698,9 +1705,11 @@
         <v>51</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="32" t="s">
         <v>47</v>
       </c>
       <c r="J11" s="15"/>
@@ -1726,9 +1735,11 @@
         <v>51</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="32" t="s">
         <v>48</v>
       </c>
       <c r="J12" s="15"/>
@@ -1754,9 +1765,11 @@
         <v>51</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="G13" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="32" t="s">
         <v>48</v>
       </c>
       <c r="J13" s="15"/>
@@ -1782,9 +1795,11 @@
         <v>51</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="32" t="s">
         <v>47</v>
       </c>
       <c r="J14" s="15"/>
@@ -1810,9 +1825,11 @@
         <v>51</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="32" t="s">
         <v>48</v>
       </c>
       <c r="J15" s="15"/>

</xml_diff>